<commit_message>
Updated file - top 5 highlighted
</commit_message>
<xml_diff>
--- a/Final results ST edit.xlsx
+++ b/Final results ST edit.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotttasker/Documents/Birkbeck/aml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC30D496-9AB1-1541-92DA-6FB3C3C53CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D07FF3A-16DB-2847-8D45-D280CDFE8C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" xr2:uid="{732B8F10-4427-2A4C-A9DC-F3BB44E8F1DC}"/>
+    <workbookView xWindow="30580" yWindow="4680" windowWidth="25600" windowHeight="14600" xr2:uid="{732B8F10-4427-2A4C-A9DC-F3BB44E8F1DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Comparator algorithims" sheetId="2" r:id="rId2"/>
+    <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Top 10" sheetId="4" r:id="rId2"/>
+    <sheet name="Computation time" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparator algorithims" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Computation time'!$A$1:$G$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Top 10'!$B$2:$P$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="96">
   <si>
     <t>Preprocessing</t>
   </si>
@@ -103,9 +109,6 @@
     <t>False Negative</t>
   </si>
   <si>
-    <t>F1score = 2*((Precision*Recall) / sum(Precision, Recall))</t>
-  </si>
-  <si>
     <t>recall (or sensitivity) = TP / (TP + FN)</t>
   </si>
   <si>
@@ -241,9 +244,6 @@
     <t xml:space="preserve">Recall/Sensitivity/Detection Rate </t>
   </si>
   <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>0,0</t>
   </si>
   <si>
@@ -257,13 +257,86 @@
   </si>
   <si>
     <t>MCC</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>FAR = fp/(tn+fp)</t>
+  </si>
+  <si>
+    <t>RBS RFE, logistic classifier, 10 features, DT, Default</t>
+  </si>
+  <si>
+    <t>RBS RFE, logistic classifier, 10 features, DT, tuned</t>
+  </si>
+  <si>
+    <t>RBS  RFE, logistic classifier, 10 features RF default</t>
+  </si>
+  <si>
+    <t>RBS  RFE, logistic classifier, 10 features RF tuned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBS  RFE, logistic classifier, 10 features KNN tuned </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specificity </t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>F1score</t>
+  </si>
+  <si>
+    <t>F1score = (2* True Positive)/((2*True Positive)+False Positive+False Negative)</t>
+  </si>
+  <si>
+    <t>False Alarm Rate</t>
+  </si>
+  <si>
+    <t>Michaels Correlation Coefficent</t>
+  </si>
+  <si>
+    <t>RFE, logistic classifier, 10 most important features</t>
+  </si>
+  <si>
+    <t>RFE, logistic classifier, 5 most important features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robust Scaler RFElog 10 DT tuned </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robust Scaler RFElog 10 DT default </t>
+  </si>
+  <si>
+    <t>Robust Scaler RFElog 10 RF default</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robust Scaler RFElog 10 RF tuned</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robust Scaler RFElog 10 KNN tuned</t>
+  </si>
+  <si>
+    <t>Time taken to test model (s)</t>
+  </si>
+  <si>
+    <t>Time taken to build model(s)</t>
+  </si>
+  <si>
+    <t>Rank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -317,8 +390,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,8 +424,14 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -352,11 +439,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -389,11 +511,73 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -411,7 +595,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -449,7 +656,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -469,6 +675,45 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -758,40 +1003,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8D4C7800-C874-4148-B61E-5C126E9C09D9}" name="Table3" displayName="Table3" ref="B2:Q98" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8D4C7800-C874-4148-B61E-5C126E9C09D9}" name="Table3" displayName="Table3" ref="B2:Q98" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B2:Q98" xr:uid="{B6711CCB-0AA5-E642-8F24-4E26F90ACA8C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q98">
     <sortCondition ref="J2:J98"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{BAE84B0C-6CC5-DE41-94E7-182E0F0F159F}" name="Preprocessing" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{41CE1890-A9EA-3A4F-9F41-3829BFA63000}" name="FeatureSelection" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{2134ACA5-764B-9340-A477-2FFE8AF18F70}" name="Algorithms " dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{1BF0B449-C87B-8645-AB85-678198323194}" name="Tuning" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{49DC004E-1B0C-0645-BF84-A2563E03AD0F}" name="Accuracy" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{A37BD30E-C75A-C54C-8EBA-ECB552F93498}" name="True Positive" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{303CF504-AB64-4748-9DF7-619D2457F830}" name="True Negative" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{0FFD8ED6-719C-6F44-8EF6-276250C9CD11}" name="False Positive" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{310B6CC9-1826-6247-AE88-117FCD767D85}" name="False Negative" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{0A0693A3-6FD8-DD4C-BB5F-FC81AAB7C345}" name="specificity = TN/(TN+FP)" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{BAE84B0C-6CC5-DE41-94E7-182E0F0F159F}" name="Preprocessing" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{41CE1890-A9EA-3A4F-9F41-3829BFA63000}" name="FeatureSelection" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2134ACA5-764B-9340-A477-2FFE8AF18F70}" name="Algorithms " dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{1BF0B449-C87B-8645-AB85-678198323194}" name="Tuning" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{49DC004E-1B0C-0645-BF84-A2563E03AD0F}" name="Accuracy" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{A37BD30E-C75A-C54C-8EBA-ECB552F93498}" name="True Positive" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{303CF504-AB64-4748-9DF7-619D2457F830}" name="True Negative" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{0FFD8ED6-719C-6F44-8EF6-276250C9CD11}" name="False Positive" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{310B6CC9-1826-6247-AE88-117FCD767D85}" name="False Negative" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{0A0693A3-6FD8-DD4C-BB5F-FC81AAB7C345}" name="specificity = TN/(TN+FP)" dataDxfId="11">
       <calculatedColumnFormula>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{12EB5B80-A723-9A46-8849-DCF02FCCC943}" name="recall (or sensitivity) = TP / (TP + FN)" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{12EB5B80-A723-9A46-8849-DCF02FCCC943}" name="recall (or sensitivity) = TP / (TP + FN)" dataDxfId="12">
       <calculatedColumnFormula>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{71DBA9EB-129D-FA4E-8047-5361EF44A233}" name="precision = TP / (TP + FP)" dataDxfId="3">
+    <tableColumn id="17" xr3:uid="{71DBA9EB-129D-FA4E-8047-5361EF44A233}" name="precision = TP / (TP + FP)" dataDxfId="10">
       <calculatedColumnFormula>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{4B19D647-F92D-B34A-B9A7-2E5F10D9EACC}" name="F1score = 2*((Precision*Recall) / sum(Precision, Recall))" dataDxfId="5">
-      <calculatedColumnFormula>2*((K3*L3)/SUM(K3,L3))</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{4B19D647-F92D-B34A-B9A7-2E5F10D9EACC}" name="F1score = (2* True Positive)/((2*True Positive)+False Positive+False Negative)" dataDxfId="6">
+      <calculatedColumnFormula>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AE1C756C-93B2-FB4F-9220-7EFF1184C6AE}" name="False Positives Rate = FP/(FP+TN)" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{AE1C756C-93B2-FB4F-9220-7EFF1184C6AE}" name="False Positives Rate = FP/(FP+TN)" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6DF92308-F06E-B24F-9490-60D6A412BADB}" name="MCC" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{6DF92308-F06E-B24F-9490-60D6A412BADB}" name="MCC" dataDxfId="8">
       <calculatedColumnFormula>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{3EFAE08C-442D-FD46-9F1B-C825276AE5D3}" name="Column2" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{3EFAE08C-442D-FD46-9F1B-C825276AE5D3}" name="FAR = fp/(tn+fp)" dataDxfId="7">
+      <calculatedColumnFormula>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B668CD09-CAF8-DC49-AEAA-A28577DE8FD8}" name="Table1" displayName="Table1" ref="B3:E8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="B3:E8" xr:uid="{CD05D9E8-FB92-7745-8B40-F1912A2A6AA5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:E8">
+    <sortCondition ref="E3:E8"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="4" xr3:uid="{9CF1309A-971A-B44C-AD6D-19E47C3A2F5A}" name="Rank" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8DAEB101-F7CD-F24E-8759-8D71B947A05F}" name="Model" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4CCF48E9-6021-A846-B367-1DDBC49165D2}" name="Time taken to build model(s)" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{066C33E4-E73D-2B46-B4B9-B5A452D58E2F}" name="Time taken to test model (s)" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{53FAB23C-0753-2741-9470-F428B75066B1}" name="Table2" displayName="Table2" ref="B50:D60" totalsRowShown="0">
+  <autoFilter ref="B50:D60" xr:uid="{C69222D4-B2F0-1B46-9ABC-B2F640491E84}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B51:D60">
+    <sortCondition descending="1" ref="C50:C60"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{219D6324-081A-2E40-BFD2-2DA272796601}" name="Model"/>
+    <tableColumn id="2" xr3:uid="{9B418C66-9DE5-5744-828A-DEA82982E324}" name="Sensitivity"/>
+    <tableColumn id="3" xr3:uid="{553A6A2B-5516-2048-90F5-675A00943C0C}" name="False Alarm Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1096,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92672284-F3C4-BD4A-AFA6-769864A7B502}">
   <dimension ref="A1:X104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,7 +1383,7 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" style="1" customWidth="1"/>
@@ -1116,7 +1394,7 @@
     <col min="12" max="12" width="27.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="24" style="1" customWidth="1"/>
     <col min="14" max="14" width="51.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" style="15" customWidth="1"/>
+    <col min="15" max="15" width="36.6640625" style="15" customWidth="1"/>
     <col min="16" max="16" width="23.5" style="1" customWidth="1"/>
     <col min="17" max="17" width="28.5" style="1" customWidth="1"/>
     <col min="18" max="21" width="10.83203125" style="1"/>
@@ -1131,7 +1409,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="L1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -1168,140 +1446,146 @@
         <v>22</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="P2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="6"/>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="14">
         <v>0.97614423029035302</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="23">
         <v>20076</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="23">
         <v>19124</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="23">
         <v>955</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="23">
         <v>3</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="11">
         <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.99984315365713394</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="11">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.99985059016883315</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="11">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
         <v>0.95459084209024769</v>
       </c>
-      <c r="N3" s="1">
-        <f>2*((K3*L3)/SUM(K3,L3))</f>
-        <v>0.999846871899156</v>
-      </c>
-      <c r="O3" s="16">
+      <c r="N3" s="11">
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O3" s="17">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
         <v>4.7562129588126896E-2</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="23">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.97695136631632318</v>
       </c>
-      <c r="Q3" s="7"/>
+      <c r="Q3" s="23">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.7562129588126896E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="14">
         <v>0.97614423029035302</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="11">
         <v>20076</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="11">
         <v>19124</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="11">
         <v>955</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="11">
         <v>3</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="11">
         <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.99984315365713394</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="11">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.99985059016883315</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="11">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
         <v>0.95459084209024769</v>
       </c>
-      <c r="N4" s="1">
-        <f>2*((K4*L4)/SUM(K4,L4))</f>
-        <v>0.999846871899156</v>
-      </c>
-      <c r="O4" s="16">
+      <c r="N4" s="11">
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O4" s="17">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
         <v>4.7562129588126896E-2</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="23">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.97695136631632318</v>
       </c>
-      <c r="Q4" s="7"/>
+      <c r="Q4" s="23">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.7562129588126896E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -1344,128 +1628,138 @@
         <v>0.95459084209024769</v>
       </c>
       <c r="N5" s="11">
-        <f>2*((K5*L5)/SUM(K5,L5))</f>
-        <v>0.999846871899156</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97669666747749939</v>
       </c>
       <c r="O5" s="17">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
         <v>4.7562129588126896E-2</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="23">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.97695136631632318</v>
       </c>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="23">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.7562129588126896E-2</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="13">
-        <v>0.97552168932715699</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="F6" s="14">
+        <v>0.97614423029035302</v>
+      </c>
+      <c r="G6" s="11">
         <v>20076</v>
       </c>
-      <c r="H6" s="1">
-        <v>19099</v>
-      </c>
-      <c r="I6" s="4">
-        <v>980</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="H6" s="11">
+        <v>19124</v>
+      </c>
+      <c r="I6" s="11">
+        <v>955</v>
+      </c>
+      <c r="J6" s="11">
         <v>3</v>
       </c>
-      <c r="K6" s="1">
-        <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.99984294838236831</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="K6" s="11">
+        <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.99984315365713394</v>
+      </c>
+      <c r="L6" s="11">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.99985059016883315</v>
       </c>
-      <c r="M6" s="1">
-        <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
-        <v>0.95345744680851063</v>
-      </c>
-      <c r="N6" s="1">
-        <f>2*((K6*L6)/SUM(K6,L6))</f>
-        <v>0.99984676926099925</v>
-      </c>
-      <c r="O6" s="16">
-        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
-        <v>4.8807211514517654E-2</v>
-      </c>
-      <c r="P6" s="4">
-        <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.9763710214638891</v>
-      </c>
-      <c r="Q6" s="7"/>
+      <c r="M6" s="11">
+        <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.95459084209024769</v>
+      </c>
+      <c r="N6" s="11">
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O6" s="24">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
+        <v>4.7562129588126896E-2</v>
+      </c>
+      <c r="P6" s="11">
+        <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97695136631632318</v>
+      </c>
+      <c r="Q6" s="11">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.7562129588126896E-2</v>
+      </c>
       <c r="R6" s="4"/>
       <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13">
-        <v>0.97509836147218398</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="14">
+        <v>0.97552168932715699</v>
+      </c>
+      <c r="G7" s="23">
         <v>20076</v>
       </c>
-      <c r="H7" s="1">
-        <v>19082</v>
-      </c>
-      <c r="I7" s="1">
-        <v>997</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="H7" s="11">
+        <v>19099</v>
+      </c>
+      <c r="I7" s="23">
+        <v>980</v>
+      </c>
+      <c r="J7" s="11">
         <v>3</v>
       </c>
-      <c r="K7" s="1">
-        <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.99984280848834162</v>
-      </c>
-      <c r="L7" s="1">
+      <c r="K7" s="11">
+        <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.99984294838236831</v>
+      </c>
+      <c r="L7" s="11">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.99985059016883315</v>
       </c>
-      <c r="M7" s="1">
-        <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
-        <v>0.95268827409481327</v>
-      </c>
-      <c r="N7" s="1">
-        <f>2*((K7*L7)/SUM(K7,L7))</f>
-        <v>0.99984669931344639</v>
-      </c>
-      <c r="O7" s="15">
-        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
-        <v>4.9653867224463369E-2</v>
-      </c>
-      <c r="P7" s="1">
-        <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.97597697663514571</v>
+      <c r="M7" s="11">
+        <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.95345744680851063</v>
+      </c>
+      <c r="N7" s="11">
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97610307524006323</v>
+      </c>
+      <c r="O7" s="17">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
+        <v>4.8807211514517654E-2</v>
+      </c>
+      <c r="P7" s="23">
+        <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.9763710214638891</v>
+      </c>
+      <c r="Q7" s="23">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.8807211514517654E-2</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -1483,26 +1777,26 @@
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="13">
-        <v>0.96269734548533203</v>
+        <v>0.97509836147218398</v>
       </c>
       <c r="G8" s="1">
         <v>20076</v>
       </c>
       <c r="H8" s="1">
-        <v>18584</v>
+        <v>19082</v>
       </c>
       <c r="I8" s="1">
-        <v>1495</v>
+        <v>997</v>
       </c>
       <c r="J8" s="1">
         <v>3</v>
       </c>
       <c r="K8" s="1">
         <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.99983859686877929</v>
+        <v>0.99984280848834162</v>
       </c>
       <c r="L8" s="1">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</f>
@@ -1510,19 +1804,23 @@
       </c>
       <c r="M8" s="1">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
-        <v>0.93069398729776087</v>
+        <v>0.95268827409481327</v>
       </c>
       <c r="N8" s="1">
-        <f>2*((K8*L8)/SUM(K8,L8))</f>
-        <v>0.99984459348284083</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97569984447900471</v>
       </c>
       <c r="O8" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
-        <v>7.4455899198167239E-2</v>
+        <v>4.9653867224463369E-2</v>
       </c>
       <c r="P8" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.96464115594588085</v>
+        <v>0.97597697663514571</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.9653867224463369E-2</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1536,49 +1834,53 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="13">
-        <v>0.97452562378604501</v>
+        <v>0.96269734548533203</v>
       </c>
       <c r="G9" s="1">
-        <v>20073</v>
+        <v>20076</v>
       </c>
       <c r="H9" s="1">
-        <v>19062</v>
+        <v>18584</v>
       </c>
       <c r="I9" s="1">
-        <v>1017</v>
+        <v>1495</v>
       </c>
       <c r="J9" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K9" s="1">
         <f>Table3[[#This Row],[True Negative]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.99968533668974202</v>
+        <v>0.99983859686877929</v>
       </c>
       <c r="L9" s="1">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.9997011803376662</v>
+        <v>0.99985059016883315</v>
       </c>
       <c r="M9" s="1">
         <f>Table3[[#This Row],[True Positive]]/(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])</f>
-        <v>0.95177809388335699</v>
+        <v>0.93069398729776087</v>
       </c>
       <c r="N9" s="1">
-        <f>2*((K9*L9)/SUM(K9,L9))</f>
-        <v>0.9996932584509296</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.96403361344537819</v>
       </c>
       <c r="O9" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
-        <v>5.0649932765575972E-2</v>
+        <v>7.4455899198167239E-2</v>
       </c>
       <c r="P9" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
-        <v>0.97542982125146349</v>
+        <v>0.96464115594588085</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.4455899198167239E-2</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1625,8 +1927,8 @@
         <v>0.93059805285118224</v>
       </c>
       <c r="N10" s="1">
-        <f>2*((K10*L10)/SUM(K10,L10))</f>
-        <v>0.99968919557712643</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.96391269898436938</v>
       </c>
       <c r="O10" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1635,6 +1937,10 @@
       <c r="P10" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.96450773288326186</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.4555505752278498E-2</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -1642,7 +1948,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -1681,8 +1987,8 @@
         <v>0.96871832005792902</v>
       </c>
       <c r="N11" s="1">
-        <f>2*((K11*L11)/SUM(K11,L11))</f>
-        <v>0.99939258588934021</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.98382115016914251</v>
       </c>
       <c r="O11" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1691,6 +1997,10 @@
       <c r="P11" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.98392111576503816</v>
+      </c>
+      <c r="Q11" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>3.227252353204841E-2</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -1698,7 +2008,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
@@ -1737,8 +2047,8 @@
         <v>0.95931733435318867</v>
       </c>
       <c r="N12" s="1">
-        <f>2*((K12*L12)/SUM(K12,L12))</f>
-        <v>0.99938932985591433</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.97894967924482279</v>
       </c>
       <c r="O12" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1747,14 +2057,18 @@
       <c r="P12" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.97912882718702698</v>
+      </c>
+      <c r="Q12" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.2382588774341354E-2</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -1793,8 +2107,8 @@
         <v>0.87371538059571507</v>
       </c>
       <c r="N13" s="1">
-        <f>2*((K13*L13)/SUM(K13,L13))</f>
-        <v>0.99919027281690131</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93227702530028111</v>
       </c>
       <c r="O13" s="16">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1804,7 +2118,10 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93426030498294499</v>
       </c>
-      <c r="Q13" s="7"/>
+      <c r="Q13" s="4">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.14442950346132777</v>
+      </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
@@ -1850,8 +2167,8 @@
         <v>0.97814740744353934</v>
       </c>
       <c r="N14" s="1">
-        <f>2*((K14*L14)/SUM(K14,L14))</f>
-        <v>0.99869121518926285</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.98831936914736318</v>
       </c>
       <c r="O14" s="16">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1861,14 +2178,17 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.98834356874540752</v>
       </c>
-      <c r="Q14" s="7"/>
+      <c r="Q14" s="4">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.2311868120922358E-2</v>
+      </c>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -1907,8 +2227,8 @@
         <v>0.93600336087382718</v>
       </c>
       <c r="N15" s="1">
-        <f>2*((K15*L15)/SUM(K15,L15))</f>
-        <v>0.99860707696898798</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.96631487639149916</v>
       </c>
       <c r="O15" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1917,6 +2237,10 @@
       <c r="P15" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.96672657001501139</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.8280292843269086E-2</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
@@ -1924,7 +2248,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -1963,8 +2287,8 @@
         <v>0.87725363206721507</v>
       </c>
       <c r="N16" s="10">
-        <f>2*((K16*L16)/SUM(K16,L16))</f>
-        <v>0.99827859639279326</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93391721599776389</v>
       </c>
       <c r="O16" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -1973,6 +2297,10 @@
       <c r="P16" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93562896380535532</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.13969819214104287</v>
       </c>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
@@ -1980,7 +2308,7 @@
     </row>
     <row r="17" spans="2:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>3</v>
@@ -2019,8 +2347,8 @@
         <v>0.96465376095540789</v>
       </c>
       <c r="N17" s="1">
-        <f>2*((K17*L17)/SUM(K17,L17))</f>
-        <v>0.99761778133192003</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.98087893254988368</v>
       </c>
       <c r="O17" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2029,6 +2357,10 @@
       <c r="P17" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.98093037527940508</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>3.6555605358832614E-2</v>
       </c>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -2036,7 +2368,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
@@ -2075,8 +2407,8 @@
         <v>0.96363286511448909</v>
       </c>
       <c r="N18" s="1">
-        <f>2*((K18*L18)/SUM(K18,L18))</f>
-        <v>0.99761640483571457</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.98035089436464629</v>
       </c>
       <c r="O18" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2085,6 +2417,10 @@
       <c r="P18" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.98040845858135817</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>3.7651277454056477E-2</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -2092,7 +2428,7 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
@@ -2131,8 +2467,8 @@
         <v>0.9294467137021909</v>
       </c>
       <c r="N19" s="1">
-        <f>2*((K19*L19)/SUM(K19,L19))</f>
-        <v>0.99715301561333802</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.9621603440405545</v>
       </c>
       <c r="O19" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2141,6 +2477,10 @@
       <c r="P19" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.96254029080179238</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.5700981124557989E-2</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
@@ -2187,8 +2527,8 @@
         <v>0.97178974083654646</v>
       </c>
       <c r="N20" s="1">
-        <f>2*((K20*L20)/SUM(K20,L20))</f>
-        <v>0.99154583730800727</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.98161112206665357</v>
       </c>
       <c r="O20" s="16">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2198,20 +2538,23 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.98141575880524679</v>
       </c>
-      <c r="Q20" s="7"/>
+      <c r="Q20" s="4">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.8786294138154291E-2</v>
+      </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>16</v>
@@ -2244,8 +2587,8 @@
         <v>0.90774193548387094</v>
       </c>
       <c r="N21" s="1">
-        <f>2*((K21*L21)/SUM(K21,L21))</f>
-        <v>0.98019103932331542</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.94296177505445322</v>
       </c>
       <c r="O21" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2254,6 +2597,10 @@
       <c r="P21" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.94165089709305461</v>
+      </c>
+      <c r="Q21" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>9.9706160665371787E-2</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -2300,8 +2647,8 @@
         <v>0.98387778834971984</v>
       </c>
       <c r="N22" s="1">
-        <f>2*((K22*L22)/SUM(K22,L22))</f>
-        <v>0.92897955391646792</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.95458625022437626</v>
       </c>
       <c r="O22" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2310,6 +2657,10 @@
       <c r="P22" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.95384938323561497</v>
+      </c>
+      <c r="Q22" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>1.5189999501967229E-2</v>
       </c>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
@@ -2356,8 +2707,8 @@
         <v>0.98387778834971984</v>
       </c>
       <c r="N23" s="1">
-        <f>2*((K23*L23)/SUM(K23,L23))</f>
-        <v>0.92897955391646792</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.95458625022437626</v>
       </c>
       <c r="O23" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2366,6 +2717,10 @@
       <c r="P23" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.95384938323561497</v>
+      </c>
+      <c r="Q23" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>1.5189999501967229E-2</v>
       </c>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
@@ -2373,13 +2728,13 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>16</v>
@@ -2412,8 +2767,8 @@
         <v>0.96131597975415761</v>
       </c>
       <c r="N24" s="10">
-        <f>2*((K24*L24)/SUM(K24,L24))</f>
-        <v>0.92824532837409579</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.94384016632438328</v>
       </c>
       <c r="O24" s="16">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2422,6 +2777,10 @@
       <c r="P24" s="4">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.9411152004213158</v>
+      </c>
+      <c r="Q24" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>3.7302654514667064E-2</v>
       </c>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
@@ -2468,8 +2827,8 @@
         <v>0.90910422975481098</v>
       </c>
       <c r="N25" s="1">
-        <f>2*((K25*L25)/SUM(K25,L25))</f>
-        <v>0.92625525235673922</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.91795921386827117</v>
       </c>
       <c r="O25" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2478,6 +2837,10 @@
       <c r="P25" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.91061679699809395</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>9.268389860052792E-2</v>
       </c>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
@@ -2524,8 +2887,8 @@
         <v>0.94847094801223242</v>
       </c>
       <c r="N26" s="1">
-        <f>2*((K26*L26)/SUM(K26,L26))</f>
-        <v>0.92760654880219318</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93750472304088261</v>
       </c>
       <c r="O26" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2534,6 +2897,10 @@
       <c r="P26" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93364055566940007</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.0351113103242195E-2</v>
       </c>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
@@ -2580,8 +2947,8 @@
         <v>0.94847094801223242</v>
       </c>
       <c r="N27" s="1">
-        <f>2*((K27*L27)/SUM(K27,L27))</f>
-        <v>0.92760654880219318</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93750472304088261</v>
       </c>
       <c r="O27" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2590,6 +2957,10 @@
       <c r="P27" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93364055566940007</v>
+      </c>
+      <c r="Q27" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.0351113103242195E-2</v>
       </c>
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
@@ -2636,8 +3007,8 @@
         <v>0.94847094801223242</v>
       </c>
       <c r="N28" s="1">
-        <f>2*((K28*L28)/SUM(K28,L28))</f>
-        <v>0.92760654880219318</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93750472304088261</v>
       </c>
       <c r="O28" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2646,6 +3017,10 @@
       <c r="P28" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93364055566940007</v>
+      </c>
+      <c r="Q28" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.0351113103242195E-2</v>
       </c>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
@@ -2692,8 +3067,8 @@
         <v>0.94847094801223242</v>
       </c>
       <c r="N29" s="1">
-        <f>2*((K29*L29)/SUM(K29,L29))</f>
-        <v>0.92760654880219318</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93750472304088261</v>
       </c>
       <c r="O29" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2702,6 +3077,10 @@
       <c r="P29" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93364055566940007</v>
+      </c>
+      <c r="Q29" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.0351113103242195E-2</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
@@ -2748,8 +3127,8 @@
         <v>1</v>
       </c>
       <c r="N30" s="1">
-        <f>2*((K30*L30)/SUM(K30,L30))</f>
-        <v>0.92913995980612152</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.96192322605661107</v>
       </c>
       <c r="O30" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2758,6 +3137,10 @@
       <c r="P30" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.96262130295202142</v>
+      </c>
+      <c r="Q30" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
       </c>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -2804,8 +3187,8 @@
         <v>1</v>
       </c>
       <c r="N31" s="1">
-        <f>2*((K31*L31)/SUM(K31,L31))</f>
-        <v>0.92913995980612152</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.96192322605661107</v>
       </c>
       <c r="O31" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2814,6 +3197,10 @@
       <c r="P31" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.96262130295202142</v>
+      </c>
+      <c r="Q31" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
       </c>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
@@ -2860,8 +3247,8 @@
         <v>0.9851742031134173</v>
       </c>
       <c r="N32" s="1">
-        <f>2*((K32*L32)/SUM(K32,L32))</f>
-        <v>0.92869235117314286</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.95501090722443216</v>
       </c>
       <c r="O32" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2871,8 +3258,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.95438910684703071</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q32" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>1.3944917575576473E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
@@ -2913,8 +3304,8 @@
         <v>0.97679546409071816</v>
       </c>
       <c r="N33" s="1">
-        <f>2*((K33*L33)/SUM(K33,L33))</f>
-        <v>0.92842775147036549</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.95105681498709327</v>
       </c>
       <c r="O33" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2924,8 +3315,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.94969182973986854</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q33" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.2013048458588574E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>1</v>
       </c>
@@ -2966,8 +3361,8 @@
         <v>0.97408512643317102</v>
       </c>
       <c r="N34" s="1">
-        <f>2*((K34*L34)/SUM(K34,L34))</f>
-        <v>0.92834026772206124</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.94977029096477794</v>
       </c>
       <c r="O34" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -2977,16 +3372,20 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.94816521324289471</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q34" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.4652622142536978E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>16</v>
@@ -3019,8 +3418,8 @@
         <v>0.95356703567035672</v>
       </c>
       <c r="N35" s="1">
-        <f>2*((K35*L35)/SUM(K35,L35))</f>
-        <v>0.92764602301689825</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93991058573918318</v>
       </c>
       <c r="O35" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3030,8 +3429,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93649042266735727</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q35" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.5121769012401017E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
@@ -3072,8 +3475,8 @@
         <v>0.94759358288770057</v>
       </c>
       <c r="N36" s="1">
-        <f>2*((K36*L36)/SUM(K36,L36))</f>
-        <v>0.92743264116780122</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93699954675932917</v>
       </c>
       <c r="O36" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3083,8 +3486,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93305095075092737</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q36" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.124757209024354E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
@@ -3125,8 +3532,8 @@
         <v>0.9474488237091353</v>
       </c>
       <c r="N37" s="1">
-        <f>2*((K37*L37)/SUM(K37,L37))</f>
-        <v>0.92742740353864805</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93692877105521566</v>
       </c>
       <c r="O37" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3136,8 +3543,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93296736451355811</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q37" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.1396981921410428E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
@@ -3178,8 +3589,8 @@
         <v>0.9474488237091353</v>
       </c>
       <c r="N38" s="1">
-        <f>2*((K38*L38)/SUM(K38,L38))</f>
-        <v>0.92742740353864805</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.93692877105521566</v>
       </c>
       <c r="O38" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3189,8 +3600,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.93296736451355811</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q38" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.1396981921410428E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
@@ -3231,8 +3646,8 @@
         <v>0.93994730069244437</v>
       </c>
       <c r="N39" s="1">
-        <f>2*((K39*L39)/SUM(K39,L39))</f>
-        <v>0.78210641687000304</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.84284850815978896</v>
       </c>
       <c r="O39" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3242,8 +3657,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.83394581846073168</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q39" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.8807211514517654E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -3284,8 +3703,8 @@
         <v>0.83330616680249936</v>
       </c>
       <c r="N40" s="1">
-        <f>2*((K40*L40)/SUM(K40,L40))</f>
-        <v>0.77281313399318641</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.7970585178255899</v>
       </c>
       <c r="O40" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3295,8 +3714,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.75332512227021631</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q40" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.15279645400667363</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
@@ -3337,8 +3760,8 @@
         <v>0.81827882409432851</v>
       </c>
       <c r="N41" s="1">
-        <f>2*((K41*L41)/SUM(K41,L41))</f>
-        <v>0.77112927258591202</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.79011900468806351</v>
       </c>
       <c r="O41" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3348,8 +3771,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.74065265279298298</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q41" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.16962996165147667</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>1</v>
       </c>
@@ -3390,8 +3817,8 @@
         <v>0.85795804195804193</v>
       </c>
       <c r="N42" s="1">
-        <f>2*((K42*L42)/SUM(K42,L42))</f>
-        <v>0.77528911971278769</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.80813616483111139</v>
       </c>
       <c r="O42" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3401,8 +3828,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.77326187012038405</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q42" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.12645052044424523</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
@@ -3443,8 +3874,8 @@
         <v>0.93207014714775249</v>
       </c>
       <c r="N43" s="1">
-        <f>2*((K43*L43)/SUM(K43,L43))</f>
-        <v>0.72124904114103139</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.79354727990389562</v>
       </c>
       <c r="O43" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3454,8 +3885,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.78342133384149937</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q43" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.0351113103242195E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>1</v>
       </c>
@@ -3496,8 +3931,8 @@
         <v>0.93207014714775249</v>
       </c>
       <c r="N44" s="1">
-        <f>2*((K44*L44)/SUM(K44,L44))</f>
-        <v>0.72124904114103139</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.79354727990389562</v>
       </c>
       <c r="O44" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3507,10 +3942,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.78342133384149937</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q44" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.0351113103242195E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
@@ -3549,8 +3988,8 @@
         <v>0.15453210239194293</v>
       </c>
       <c r="N45" s="1">
-        <f>2*((K45*L45)/SUM(K45,L45))</f>
-        <v>0.12361485922734838</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>9.9490054371686204E-2</v>
       </c>
       <c r="O45" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3560,10 +3999,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.79523645559482348</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q45" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.40136460979132427</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -3602,8 +4045,8 @@
         <v>0.15415226725311551</v>
       </c>
       <c r="N46" s="1">
-        <f>2*((K46*L46)/SUM(K46,L46))</f>
-        <v>0.1235257972317786</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>9.936546510058053E-2</v>
       </c>
       <c r="O46" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3613,10 +4056,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.79801543593772362</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q46" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.40226106877832563</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>5</v>
@@ -3655,8 +4102,8 @@
         <v>0.11790182868142444</v>
       </c>
       <c r="N47" s="1">
-        <f>2*((K47*L47)/SUM(K47,L47))</f>
-        <v>0.11970021802963401</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>9.0330906074292561E-2</v>
       </c>
       <c r="O47" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3666,10 +4113,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-1.3314986020521025</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q47" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.5477364410578216</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>5</v>
@@ -3708,8 +4159,8 @@
         <v>7.9422577854671286E-2</v>
       </c>
       <c r="N48" s="1">
-        <f>2*((K48*L48)/SUM(K48,L48))</f>
-        <v>9.6310708276137455E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>7.616331821127674E-2</v>
       </c>
       <c r="O48" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3719,10 +4170,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-5.3113065255445742</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q48" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.84800039842621644</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>5</v>
@@ -3761,8 +4216,8 @@
         <v>7.9405405405405402E-2</v>
       </c>
       <c r="N49" s="1">
-        <f>2*((K49*L49)/SUM(K49,L49))</f>
-        <v>9.6273609574673472E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>7.6155421343217816E-2</v>
       </c>
       <c r="O49" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3772,10 +4227,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-5.3190689582902193</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q49" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.84819961153443901</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>6</v>
@@ -3814,8 +4273,8 @@
         <v>0.91180124223602488</v>
       </c>
       <c r="N50" s="1">
-        <f>2*((K50*L50)/SUM(K50,L50))</f>
-        <v>0.12811246502918461</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13536815897459542</v>
       </c>
       <c r="O50" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3825,10 +4284,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23487771703461846</v>
       </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q50" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.0720653418994972E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
@@ -3867,8 +4330,8 @@
         <v>0.90561381863047496</v>
       </c>
       <c r="N51" s="1">
-        <f>2*((K51*L51)/SUM(K51,L51))</f>
-        <v>0.12810823619259809</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13529953917050691</v>
       </c>
       <c r="O51" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3878,8 +4341,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23226574248335932</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q51" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.6199013895114302E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>1</v>
       </c>
@@ -3920,8 +4387,8 @@
         <v>0.99660326086956519</v>
       </c>
       <c r="N52" s="1">
-        <f>2*((K52*L52)/SUM(K52,L52))</f>
-        <v>0.1280878290056752</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13614217437705906</v>
       </c>
       <c r="O52" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3931,10 +4398,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.26898656420283668</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q52" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.490163852781513E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>3</v>
@@ -3973,8 +4444,8 @@
         <v>0.91859737006887909</v>
       </c>
       <c r="N53" s="1">
-        <f>2*((K53*L53)/SUM(K53,L53))</f>
-        <v>0.12804018895857355</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13535707695146706</v>
       </c>
       <c r="O53" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -3984,10 +4455,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23764509708158651</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q53" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.4744260172319339E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>3</v>
@@ -4026,8 +4501,8 @@
         <v>0.91401869158878501</v>
       </c>
       <c r="N54" s="1">
-        <f>2*((K54*L54)/SUM(K54,L54))</f>
-        <v>0.1280371208750562</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13530713890426121</v>
       </c>
       <c r="O54" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4037,10 +4512,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23572821569473421</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q54" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.8728522336769758E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>3</v>
@@ -4079,8 +4558,8 @@
         <v>0.91288114499066586</v>
       </c>
       <c r="N55" s="1">
-        <f>2*((K55*L55)/SUM(K55,L55))</f>
-        <v>0.12803635349248088</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13529466014940514</v>
       </c>
       <c r="O55" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4090,10 +4569,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23525055188492575</v>
       </c>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q55" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.9724587877882365E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>6</v>
@@ -4132,8 +4615,8 @@
         <v>0.91174642635177128</v>
       </c>
       <c r="N56" s="1">
-        <f>2*((K56*L56)/SUM(K56,L56))</f>
-        <v>0.12803558596514533</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.1352821836960531</v>
       </c>
       <c r="O56" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4143,10 +4626,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23477350687006862</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q56" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.0720653418994972E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>3</v>
@@ -4185,8 +4672,8 @@
         <v>0.88108108108108107</v>
       </c>
       <c r="N57" s="1">
-        <f>2*((K57*L57)/SUM(K57,L57))</f>
-        <v>0.12801403626033919</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13493377483443708</v>
       </c>
       <c r="O57" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4196,10 +4683,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.22165999426346827</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q57" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>9.8610488570147915E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>5</v>
@@ -4238,8 +4729,8 @@
         <v>0.58399681528662417</v>
       </c>
       <c r="N58" s="1">
-        <f>2*((K58*L58)/SUM(K58,L58))</f>
-        <v>0.12767359917723758</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.12987472887433049</v>
       </c>
       <c r="O58" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4249,10 +4740,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>6.2682110122843776E-2</v>
       </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q58" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.2044424523133626E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>6</v>
@@ -4291,8 +4786,8 @@
         <v>0.91101431238332298</v>
       </c>
       <c r="N59" s="1">
-        <f>2*((K59*L59)/SUM(K59,L59))</f>
-        <v>0.12780449473733496</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13501798395278058</v>
       </c>
       <c r="O59" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4302,10 +4797,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.23422211272242033</v>
       </c>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q59" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.1218686189551276E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>6</v>
@@ -4344,8 +4843,8 @@
         <v>0.76</v>
       </c>
       <c r="N60" s="1">
-        <f>2*((K60*L60)/SUM(K60,L60))</f>
-        <v>0.12760382422996844</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13297582257771315</v>
       </c>
       <c r="O60" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4355,10 +4854,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.16479998134641344</v>
       </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q60" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.3009113999701181E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
@@ -4397,8 +4900,8 @@
         <v>0.77260708619777896</v>
       </c>
       <c r="N61" s="1">
-        <f>2*((K61*L61)/SUM(K61,L61))</f>
-        <v>0.1274627749940648</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13299954483386436</v>
       </c>
       <c r="O61" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4408,10 +4911,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.17097928158631914</v>
       </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q61" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.1415409133921013E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>3</v>
@@ -4450,8 +4957,8 @@
         <v>0.97435897435897434</v>
       </c>
       <c r="N62" s="1">
-        <f>2*((K62*L62)/SUM(K62,L62))</f>
-        <v>0.12630274593192006</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13394554983535087</v>
       </c>
       <c r="O62" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4461,10 +4968,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.25823367191704044</v>
       </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q62" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>1.89252452811395E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>3</v>
@@ -4503,8 +5014,8 @@
         <v>0.96782841823056298</v>
       </c>
       <c r="N63" s="1">
-        <f>2*((K63*L63)/SUM(K63,L63))</f>
-        <v>0.12629904347310331</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13388345463817161</v>
       </c>
       <c r="O63" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4514,10 +5025,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.25566390357460134</v>
       </c>
-    </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q63" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.3905572986702523E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>3</v>
@@ -4556,8 +5071,8 @@
         <v>0.71733730750124192</v>
       </c>
       <c r="N64" s="1">
-        <f>2*((K64*L64)/SUM(K64,L64))</f>
-        <v>0.12610121147165607</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.13072605468042731</v>
       </c>
       <c r="O64" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4566,11 +5081,15 @@
       <c r="P64" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0.14164457181383916</v>
+      </c>
+      <c r="Q64" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.8338064644653618E-2</v>
       </c>
     </row>
     <row r="65" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>5</v>
@@ -4609,8 +5128,8 @@
         <v>0.38676707907477137</v>
       </c>
       <c r="N65" s="1">
-        <f>2*((K65*L65)/SUM(K65,L65))</f>
-        <v>0.12491841825638321</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.1208555700298357</v>
       </c>
       <c r="O65" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4619,11 +5138,15 @@
       <c r="P65" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.10993420375875428</v>
+      </c>
+      <c r="Q65" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.11355147168683699</v>
       </c>
     </row>
     <row r="66" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>4</v>
@@ -4662,8 +5185,8 @@
         <v>0.48725113517289559</v>
       </c>
       <c r="N66" s="10">
-        <f>2*((K66*L66)/SUM(K66,L66))</f>
-        <v>0.12197002968128147</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.12161101909162235</v>
       </c>
       <c r="O66" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4672,11 +5195,15 @@
       <c r="P66" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-1.0387559311275531E-2</v>
+      </c>
+      <c r="Q66" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>7.3111210717665229E-2</v>
       </c>
     </row>
     <row r="67" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>4</v>
@@ -4715,8 +5242,8 @@
         <v>0.60450997398091932</v>
       </c>
       <c r="N67" s="10">
-        <f>2*((K67*L67)/SUM(K67,L67))</f>
-        <v>0.12210961686176226</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.12454768818405182</v>
       </c>
       <c r="O67" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4725,11 +5252,15 @@
       <c r="P67" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>7.4205190363525714E-2</v>
+      </c>
+      <c r="Q67" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.5420588674734801E-2</v>
       </c>
     </row>
     <row r="68" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>4</v>
@@ -4768,8 +5299,8 @@
         <v>0.60178173719376393</v>
       </c>
       <c r="N68" s="10">
-        <f>2*((K68*L68)/SUM(K68,L68))</f>
-        <v>0.11877540059829794</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.12103565669234904</v>
       </c>
       <c r="O68" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4778,11 +5309,15 @@
       <c r="P68" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>7.1238909612650891E-2</v>
+      </c>
+      <c r="Q68" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.4524129687733456E-2</v>
       </c>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>4</v>
@@ -4821,8 +5356,8 @@
         <v>0.60385823239120684</v>
       </c>
       <c r="N69" s="10">
-        <f>2*((K69*L69)/SUM(K69,L69))</f>
-        <v>0.11838933331177953</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.12067419759727452</v>
       </c>
       <c r="O69" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4831,11 +5366,15 @@
       <c r="P69" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>7.2391279899971156E-2</v>
+      </c>
+      <c r="Q69" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.3976293640121518E-2</v>
       </c>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>4</v>
@@ -4874,8 +5413,8 @@
         <v>0.52379079826976016</v>
       </c>
       <c r="N70" s="10">
-        <f>2*((K70*L70)/SUM(K70,L70))</f>
-        <v>0.11717895406122943</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.11776147113429405</v>
       </c>
       <c r="O70" s="16">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4885,10 +5424,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>1.8020106868626831E-2</v>
       </c>
-    </row>
-    <row r="71" spans="2:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q70" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.0311768514368244E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>4</v>
@@ -4927,8 +5470,8 @@
         <v>0.53568532035685323</v>
       </c>
       <c r="N71" s="10">
-        <f>2*((K71*L71)/SUM(K71,L71))</f>
-        <v>0.11634296943747659</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>0.11718784652916389</v>
       </c>
       <c r="O71" s="16">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4938,7 +5481,10 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>2.6524352963472855E-2</v>
       </c>
-      <c r="Q71" s="7"/>
+      <c r="Q71" s="4">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.702475222869665E-2</v>
+      </c>
     </row>
     <row r="72" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -4981,8 +5527,8 @@
         <v>6.7600487210718638E-2</v>
       </c>
       <c r="N72" s="1">
-        <f>2*((K72*L72)/SUM(K72,L72))</f>
-        <v>6.0733412452028963E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>4.4502355417460157E-2</v>
       </c>
       <c r="O72" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -4991,6 +5537,10 @@
       <c r="P72" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-1.116608497334945</v>
+      </c>
+      <c r="Q72" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.45749290303301959</v>
       </c>
     </row>
     <row r="73" spans="2:17" x14ac:dyDescent="0.2">
@@ -5034,8 +5584,8 @@
         <v>6.7262751473277788E-2</v>
       </c>
       <c r="N73" s="1">
-        <f>2*((K73*L73)/SUM(K73,L73))</f>
-        <v>6.0400414945844104E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>4.4249857959292802E-2</v>
       </c>
       <c r="O73" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5044,6 +5594,10 @@
       <c r="P73" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-1.1162985014745435</v>
+      </c>
+      <c r="Q73" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.45719408337068579</v>
       </c>
     </row>
     <row r="74" spans="2:17" ht="19" x14ac:dyDescent="0.25">
@@ -5087,8 +5641,8 @@
         <v>0.30888290713324362</v>
       </c>
       <c r="N74" s="1">
-        <f>2*((K74*L74)/SUM(K74,L74))</f>
-        <v>4.3692056376463985E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>4.2568977509853931E-2</v>
       </c>
       <c r="O74" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5097,6 +5651,10 @@
       <c r="P74" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.10958961409577295</v>
+      </c>
+      <c r="Q74" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.1147965536132274E-2</v>
       </c>
     </row>
     <row r="75" spans="2:17" ht="19" x14ac:dyDescent="0.25">
@@ -5140,8 +5698,8 @@
         <v>0.30888290713324362</v>
       </c>
       <c r="N75" s="1">
-        <f>2*((K75*L75)/SUM(K75,L75))</f>
-        <v>4.3692056376463985E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>4.2568977509853931E-2</v>
       </c>
       <c r="O75" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5150,11 +5708,15 @@
       <c r="P75" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.10958961409577295</v>
+      </c>
+      <c r="Q75" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>5.1147965536132274E-2</v>
       </c>
     </row>
     <row r="76" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>4</v>
@@ -5193,8 +5755,8 @@
         <v>0.21732745961820851</v>
       </c>
       <c r="N76" s="10">
-        <f>2*((K76*L76)/SUM(K76,L76))</f>
-        <v>1.4525529106676151E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>1.4258188824662813E-2</v>
       </c>
       <c r="O76" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5203,6 +5765,10 @@
       <c r="P76" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.10695480950560934</v>
+      </c>
+      <c r="Q76" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.6545146670650929E-2</v>
       </c>
     </row>
     <row r="77" spans="2:17" ht="19" x14ac:dyDescent="0.25">
@@ -5246,8 +5812,8 @@
         <v>2.2300095571838166E-2</v>
       </c>
       <c r="N77" s="1">
-        <f>2*((K77*L77)/SUM(K77,L77))</f>
-        <v>1.3712561507353749E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>1.0623363812269986E-2</v>
       </c>
       <c r="O77" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5256,6 +5822,10 @@
       <c r="P77" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.76943673638506327</v>
+      </c>
+      <c r="Q77" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.30569251456745855</v>
       </c>
     </row>
     <row r="78" spans="2:17" ht="19" x14ac:dyDescent="0.25">
@@ -5299,8 +5869,8 @@
         <v>2.3840810963018585E-2</v>
       </c>
       <c r="N78" s="1">
-        <f>2*((K78*L78)/SUM(K78,L78))</f>
-        <v>1.2465461902836811E-2</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>9.9976383531449262E-3</v>
       </c>
       <c r="O78" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5309,11 +5879,15 @@
       <c r="P78" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.66194332832510172</v>
+      </c>
+      <c r="Q78" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.25897704068927735</v>
       </c>
     </row>
     <row r="79" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>4</v>
@@ -5352,8 +5926,8 @@
         <v>0.24653739612188366</v>
       </c>
       <c r="N79" s="10">
-        <f>2*((K79*L79)/SUM(K79,L79))</f>
-        <v>8.7867292690861007E-3</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>8.7084148727984336E-3</v>
       </c>
       <c r="O79" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5362,11 +5936,15 @@
       <c r="P79" s="1">
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-6.8904855555036934E-2</v>
+      </c>
+      <c r="Q79" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>1.354649135913143E-2</v>
       </c>
     </row>
     <row r="80" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>5</v>
@@ -5405,8 +5983,8 @@
         <v>4.1031036296685953E-2</v>
       </c>
       <c r="N80" s="1">
-        <f>2*((K80*L80)/SUM(K80,L80))</f>
-        <v>7.7065748762665089E-3</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>7.0973612374886259E-3</v>
       </c>
       <c r="O80" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5416,8 +5994,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.31064887493286825</v>
       </c>
-    </row>
-    <row r="81" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q80" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>9.0791374072413972E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>1</v>
       </c>
@@ -5458,8 +6040,8 @@
         <v>7.8947368421052627E-2</v>
       </c>
       <c r="N81" s="1">
-        <f>2*((K81*L81)/SUM(K81,L81))</f>
-        <v>1.1938470890932339E-3</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>1.1862982551529831E-3</v>
       </c>
       <c r="O81" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5469,16 +6051,20 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-7.3782920508436781E-2</v>
       </c>
-    </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q81" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.9724587877882365E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>15</v>
@@ -5511,8 +6097,8 @@
         <v>0.21875</v>
       </c>
       <c r="N82" s="10">
-        <f>2*((K82*L82)/SUM(K82,L82))</f>
-        <v>6.9675984781928692E-4</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>6.9613644274277764E-4</v>
       </c>
       <c r="O82" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5522,8 +6108,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-2.2483687724819443E-2</v>
       </c>
-    </row>
-    <row r="83" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q82" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>1.2450819263907565E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>1</v>
       </c>
@@ -5564,8 +6154,8 @@
         <v>1</v>
       </c>
       <c r="N83" s="1">
-        <f>2*((K83*L83)/SUM(K83,L83))</f>
-        <v>9.9596633880794723E-5</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>9.9601593625498012E-5</v>
       </c>
       <c r="O83" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5575,8 +6165,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>7.0571436808461001E-3</v>
       </c>
-    </row>
-    <row r="84" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q83" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>1</v>
       </c>
@@ -5617,8 +6211,8 @@
         <v>1.1947431302270011E-3</v>
       </c>
       <c r="N84" s="1">
-        <f>2*((K84*L84)/SUM(K84,L84))</f>
-        <v>9.9596418419009564E-5</v>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
+        <v>9.5620577548288392E-5</v>
       </c>
       <c r="O84" s="15">
         <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[False Positive]]+Table3[[#This Row],[True Negative]])</f>
@@ -5628,8 +6222,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.21253086310464556</v>
       </c>
-    </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q84" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>4.1635539618506898E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B85" s="2" t="s">
         <v>1</v>
       </c>
@@ -5670,7 +6268,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N85" s="1">
-        <f>2*((K85*L85)/SUM(K85,L85))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O85" s="15">
@@ -5681,8 +6279,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q85" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B86" s="2" t="s">
         <v>1</v>
       </c>
@@ -5723,7 +6325,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N86" s="1">
-        <f>2*((K86*L86)/SUM(K86,L86))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O86" s="15">
@@ -5734,8 +6336,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q86" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B87" s="2" t="s">
         <v>1</v>
       </c>
@@ -5776,7 +6382,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N87" s="1">
-        <f>2*((K87*L87)/SUM(K87,L87))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O87" s="15">
@@ -5787,8 +6393,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q87" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B88" s="2" t="s">
         <v>1</v>
       </c>
@@ -5829,7 +6439,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N88" s="1">
-        <f>2*((K88*L88)/SUM(K88,L88))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O88" s="15">
@@ -5840,8 +6450,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q88" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B89" s="2" t="s">
         <v>1</v>
       </c>
@@ -5882,7 +6496,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N89" s="1">
-        <f>2*((K89*L89)/SUM(K89,L89))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O89" s="15">
@@ -5893,8 +6507,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q89" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B90" s="2" t="s">
         <v>1</v>
       </c>
@@ -5935,7 +6553,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N90" s="1">
-        <f>2*((K90*L90)/SUM(K90,L90))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O90" s="15">
@@ -5946,16 +6564,20 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q90" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B91" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>15</v>
@@ -5988,7 +6610,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N91" s="1">
-        <f>2*((K91*L91)/SUM(K91,L91))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O91" s="15">
@@ -5999,16 +6621,20 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q91" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B92" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>15</v>
@@ -6041,7 +6667,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N92" s="1">
-        <f>2*((K92*L92)/SUM(K92,L92))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O92" s="15">
@@ -6052,8 +6678,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q92" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B93" s="2" t="s">
         <v>1</v>
       </c>
@@ -6094,7 +6724,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N93" s="1">
-        <f>2*((K93*L93)/SUM(K93,L93))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O93" s="15">
@@ -6105,10 +6735,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q93" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B94" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>3</v>
@@ -6147,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="N94" s="1">
-        <f>2*((K94*L94)/SUM(K94,L94))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O94" s="15">
@@ -6158,16 +6792,20 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-8.3476388004442043E-2</v>
       </c>
-    </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q94" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>6.8728522336769758E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B95" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>15</v>
@@ -6200,7 +6838,7 @@
         <v>0</v>
       </c>
       <c r="N95" s="1">
-        <f>2*((K95*L95)/SUM(K95,L95))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O95" s="15">
@@ -6211,16 +6849,20 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.16098011685527217</v>
       </c>
-    </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q95" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.4652622142536978E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B96" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>16</v>
@@ -6253,7 +6895,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="1">
-        <f>2*((K96*L96)/SUM(K96,L96))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O96" s="15">
@@ -6264,10 +6906,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.16098011685527217</v>
       </c>
-    </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q96" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>2.4652622142536978E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B97" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>5</v>
@@ -6306,7 +6952,7 @@
         <v>0</v>
       </c>
       <c r="N97" s="1">
-        <f>2*((K97*L97)/SUM(K97,L97))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O97" s="15">
@@ -6317,10 +6963,14 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.20434997158234067</v>
       </c>
-    </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q97" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>3.8597539718113451E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B98" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>5</v>
@@ -6359,7 +7009,7 @@
         <v>0</v>
       </c>
       <c r="N98" s="1">
-        <f>2*((K98*L98)/SUM(K98,L98))</f>
+        <f>(2*Table3[[#This Row],[True Positive]])/((2*Table3[[#This Row],[True Positive]])+Table3[[#This Row],[False Positive]]+Table3[[#This Row],[False Negative]])</f>
         <v>0</v>
       </c>
       <c r="O98" s="15">
@@ -6370,8 +7020,12 @@
         <f>((Table3[[#This Row],[True Positive]]*Table3[[#This Row],[True Negative]])-(Table3[[#This Row],[False Positive]]*Table3[[#This Row],[False Negative]]))/SQRT(((Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Positive]])*(Table3[[#This Row],[True Positive]]+Table3[[#This Row],[False Negative]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])*Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Negative]])</f>
         <v>-0.36783939972620078</v>
       </c>
-    </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q98" s="1">
+        <f>Table3[[#This Row],[False Positive]]/(Table3[[#This Row],[True Negative]]+Table3[[#This Row],[False Positive]])</f>
+        <v>0.10772448827132826</v>
+      </c>
+    </row>
+    <row r="104" spans="2:17" x14ac:dyDescent="0.2">
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -6399,58 +7053,794 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B0F794-30ED-E343-82A6-82079730D3BE}">
+  <dimension ref="B2:Q13"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="26" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G3" s="26">
+        <v>19124</v>
+      </c>
+      <c r="H3" s="26">
+        <v>955</v>
+      </c>
+      <c r="I3" s="26">
+        <v>3</v>
+      </c>
+      <c r="J3" s="27">
+        <v>0.97614423029035302</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L3" s="27">
+        <v>0.99984315365713394</v>
+      </c>
+      <c r="M3" s="27">
+        <v>0.95459084209024769</v>
+      </c>
+      <c r="N3" s="27">
+        <f>(2*F3)/((2*F3)+H3+I3)</f>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O3" s="27">
+        <v>4.7562129588126896E-2</v>
+      </c>
+      <c r="P3" s="27">
+        <v>0.97695136631632318</v>
+      </c>
+      <c r="Q3" s="25"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G4" s="26">
+        <v>19124</v>
+      </c>
+      <c r="H4" s="26">
+        <v>955</v>
+      </c>
+      <c r="I4" s="26">
+        <v>3</v>
+      </c>
+      <c r="J4" s="27">
+        <v>0.97614423029035302</v>
+      </c>
+      <c r="K4" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L4" s="27">
+        <v>0.99984315365713394</v>
+      </c>
+      <c r="M4" s="27">
+        <v>0.95459084209024769</v>
+      </c>
+      <c r="N4" s="27">
+        <f t="shared" ref="N4:N13" si="0">(2*F4)/((2*F4)+H4+I4)</f>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O4" s="27">
+        <v>4.7562129588126896E-2</v>
+      </c>
+      <c r="P4" s="27">
+        <v>0.97695136631632318</v>
+      </c>
+      <c r="Q4" s="25"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G5" s="26">
+        <v>19124</v>
+      </c>
+      <c r="H5" s="26">
+        <v>955</v>
+      </c>
+      <c r="I5" s="26">
+        <v>3</v>
+      </c>
+      <c r="J5" s="27">
+        <v>0.97614423029035302</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L5" s="27">
+        <v>0.99984315365713394</v>
+      </c>
+      <c r="M5" s="27">
+        <v>0.95459084209024769</v>
+      </c>
+      <c r="N5" s="27">
+        <f t="shared" si="0"/>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O5" s="27">
+        <v>4.7562129588126896E-2</v>
+      </c>
+      <c r="P5" s="27">
+        <v>0.97695136631632318</v>
+      </c>
+      <c r="Q5" s="25"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G6" s="26">
+        <v>19124</v>
+      </c>
+      <c r="H6" s="26">
+        <v>955</v>
+      </c>
+      <c r="I6" s="26">
+        <v>3</v>
+      </c>
+      <c r="J6" s="27">
+        <v>0.97614423029035302</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L6" s="27">
+        <v>0.99984315365713394</v>
+      </c>
+      <c r="M6" s="27">
+        <v>0.95459084209024769</v>
+      </c>
+      <c r="N6" s="27">
+        <f t="shared" si="0"/>
+        <v>0.97669666747749939</v>
+      </c>
+      <c r="O6" s="27">
+        <v>4.7562129588126896E-2</v>
+      </c>
+      <c r="P6" s="27">
+        <v>0.97695136631632318</v>
+      </c>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G7" s="26">
+        <v>19099</v>
+      </c>
+      <c r="H7" s="26">
+        <v>980</v>
+      </c>
+      <c r="I7" s="26">
+        <v>3</v>
+      </c>
+      <c r="J7" s="27">
+        <v>0.97552168932715699</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L7" s="27">
+        <v>0.99984294838236831</v>
+      </c>
+      <c r="M7" s="27">
+        <v>0.95345744680851063</v>
+      </c>
+      <c r="N7" s="27">
+        <f t="shared" si="0"/>
+        <v>0.97610307524006323</v>
+      </c>
+      <c r="O7" s="27">
+        <v>4.8807211514517654E-2</v>
+      </c>
+      <c r="P7" s="27">
+        <v>0.9763710214638891</v>
+      </c>
+      <c r="Q7" s="25"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G8" s="26">
+        <v>19082</v>
+      </c>
+      <c r="H8" s="26">
+        <v>997</v>
+      </c>
+      <c r="I8" s="26">
+        <v>3</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0.97509836147218398</v>
+      </c>
+      <c r="K8" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L8" s="27">
+        <v>0.99984280848834162</v>
+      </c>
+      <c r="M8" s="27">
+        <v>0.95268827409481327</v>
+      </c>
+      <c r="N8" s="27">
+        <f t="shared" si="0"/>
+        <v>0.97569984447900471</v>
+      </c>
+      <c r="O8" s="27">
+        <v>4.9653867224463369E-2</v>
+      </c>
+      <c r="P8" s="27">
+        <v>0.97597697663514571</v>
+      </c>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="26">
+        <v>20076</v>
+      </c>
+      <c r="G9" s="26">
+        <v>18584</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1495</v>
+      </c>
+      <c r="I9" s="26">
+        <v>3</v>
+      </c>
+      <c r="J9" s="27">
+        <v>0.96269734548533203</v>
+      </c>
+      <c r="K9" s="27">
+        <v>0.99985059016883315</v>
+      </c>
+      <c r="L9" s="27">
+        <v>0.99983859686877929</v>
+      </c>
+      <c r="M9" s="27">
+        <v>0.93069398729776087</v>
+      </c>
+      <c r="N9" s="27">
+        <f t="shared" si="0"/>
+        <v>0.96403361344537819</v>
+      </c>
+      <c r="O9" s="27">
+        <v>7.4455899198167239E-2</v>
+      </c>
+      <c r="P9" s="27">
+        <v>0.96464115594588085</v>
+      </c>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="26">
+        <v>20073</v>
+      </c>
+      <c r="G10" s="26">
+        <v>18582</v>
+      </c>
+      <c r="H10" s="26">
+        <v>1497</v>
+      </c>
+      <c r="I10" s="26">
+        <v>6</v>
+      </c>
+      <c r="J10" s="27">
+        <v>0.96257283729269305</v>
+      </c>
+      <c r="K10" s="27">
+        <v>0.9997011803376662</v>
+      </c>
+      <c r="L10" s="27">
+        <v>0.99967721110393803</v>
+      </c>
+      <c r="M10" s="27">
+        <v>0.93059805285118224</v>
+      </c>
+      <c r="N10" s="27">
+        <f t="shared" si="0"/>
+        <v>0.96391269898436938</v>
+      </c>
+      <c r="O10" s="27">
+        <v>7.4555505752278498E-2</v>
+      </c>
+      <c r="P10" s="27">
+        <v>0.96450773288326186</v>
+      </c>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="26">
+        <v>20067</v>
+      </c>
+      <c r="G11" s="26">
+        <v>19431</v>
+      </c>
+      <c r="H11" s="26">
+        <v>648</v>
+      </c>
+      <c r="I11" s="26">
+        <v>12</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0.98356491857164197</v>
+      </c>
+      <c r="K11" s="27">
+        <v>0.99940236067533239</v>
+      </c>
+      <c r="L11" s="27">
+        <v>0.99938281129455331</v>
+      </c>
+      <c r="M11" s="27">
+        <v>0.96871832005792902</v>
+      </c>
+      <c r="N11" s="27">
+        <f t="shared" si="0"/>
+        <v>0.98382115016914251</v>
+      </c>
+      <c r="O11" s="27">
+        <v>3.227252353204841E-2</v>
+      </c>
+      <c r="P11" s="27">
+        <v>0.98392111576503816</v>
+      </c>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="26">
+        <v>20067</v>
+      </c>
+      <c r="G12" s="26">
+        <v>19228</v>
+      </c>
+      <c r="H12" s="26">
+        <v>851</v>
+      </c>
+      <c r="I12" s="26">
+        <v>12</v>
+      </c>
+      <c r="J12" s="27">
+        <v>0.97850988595049604</v>
+      </c>
+      <c r="K12" s="27">
+        <v>0.99940236067533239</v>
+      </c>
+      <c r="L12" s="27">
+        <v>0.99937629937629935</v>
+      </c>
+      <c r="M12" s="27">
+        <v>0.95931733435318867</v>
+      </c>
+      <c r="N12" s="27">
+        <f t="shared" si="0"/>
+        <v>0.97894967924482279</v>
+      </c>
+      <c r="O12" s="27">
+        <v>4.2382588774341354E-2</v>
+      </c>
+      <c r="P12" s="27">
+        <v>0.97912882718702698</v>
+      </c>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="26">
+        <v>20064</v>
+      </c>
+      <c r="G13" s="26">
+        <v>17179</v>
+      </c>
+      <c r="H13" s="26">
+        <v>2900</v>
+      </c>
+      <c r="I13" s="26">
+        <v>15</v>
+      </c>
+      <c r="J13" s="27">
+        <v>0.927411723691419</v>
+      </c>
+      <c r="K13" s="27">
+        <v>0.99925295084416554</v>
+      </c>
+      <c r="L13" s="27">
+        <v>0.99912760265208789</v>
+      </c>
+      <c r="M13" s="27">
+        <v>0.87371538059571507</v>
+      </c>
+      <c r="N13" s="27">
+        <f t="shared" si="0"/>
+        <v>0.93227702530028111</v>
+      </c>
+      <c r="O13" s="27">
+        <v>0.14442950346132777</v>
+      </c>
+      <c r="P13" s="27">
+        <v>0.93426030498294499</v>
+      </c>
+      <c r="Q13" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="34" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5353DD0-2E46-ED42-AC6A-8CE8E266B680}">
+  <dimension ref="B3:G8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="36.5" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="32">
+        <v>4.0697813034057603E-2</v>
+      </c>
+      <c r="E4" s="33">
+        <v>4.8840045928955E-3</v>
+      </c>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="34">
+        <v>4.0223121643066399E-2</v>
+      </c>
+      <c r="E5" s="33">
+        <v>5.9170722961425703E-3</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="34">
+        <v>0.20262932777404699</v>
+      </c>
+      <c r="E6" s="33">
+        <v>3.3593177795410101E-2</v>
+      </c>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0.26797509193420399</v>
+      </c>
+      <c r="E7" s="33">
+        <v>3.8874149322509703E-2</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="35">
+        <v>1.08799934387207E-2</v>
+      </c>
+      <c r="E8" s="33">
+        <v>95.848281860351506</v>
+      </c>
+      <c r="G8" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="72" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="6" max="1048575" man="1"/>
+  </colBreaks>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB89C8D8-81DF-2342-820D-9129F72E415A}">
-  <dimension ref="A8:L41"/>
+  <dimension ref="A8:L60"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="99" customWidth="1"/>
-    <col min="2" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>36</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
         <v>37</v>
       </c>
-      <c r="H12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>27</v>
-      </c>
-      <c r="K12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>92.207300000000004</v>
@@ -6482,7 +7872,7 @@
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>92.207300000000004</v>
@@ -6514,7 +7904,7 @@
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>96.1982</v>
@@ -6546,7 +7936,7 @@
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>89.432299999999998</v>
@@ -6578,7 +7968,7 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>94.575800000000001</v>
@@ -6610,7 +8000,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>95.589100000000002</v>
@@ -6642,7 +8032,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>91.437899999999999</v>
@@ -6674,7 +8064,7 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>92.207300000000004</v>
@@ -6706,35 +8096,35 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
         <v>47</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>48</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>49</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>50</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>51</v>
-      </c>
-      <c r="I25" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>96.34</v>
@@ -6757,7 +8147,7 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28">
         <v>95.91</v>
@@ -6780,7 +8170,7 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29">
         <v>99.88</v>
@@ -6826,7 +8216,7 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31">
         <v>99.55</v>
@@ -6849,23 +8239,23 @@
     </row>
     <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B34" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
         <v>45</v>
-      </c>
-      <c r="D36" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37">
         <v>99.918000000000006</v>
@@ -6876,10 +8266,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>99.876999999999995</v>
@@ -6890,10 +8280,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39">
         <v>99.549000000000007</v>
@@ -6904,10 +8294,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40">
         <v>84.828999999999994</v>
@@ -6918,10 +8308,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41">
         <v>22.007999999999999</v>
@@ -6930,7 +8320,131 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="22">
+        <v>99.985059016883312</v>
+      </c>
+      <c r="D51" s="22">
+        <v>4.7562129588126896E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="22">
+        <v>99.985059016883312</v>
+      </c>
+      <c r="D52" s="22">
+        <v>4.7562129588126896E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="22">
+        <v>99.985059016883312</v>
+      </c>
+      <c r="D53" s="22">
+        <v>4.7562129588126896E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="22">
+        <v>99.985059016883312</v>
+      </c>
+      <c r="D54" s="22">
+        <v>4.7562129588126896E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="22">
+        <v>99.985059016883312</v>
+      </c>
+      <c r="D55" s="22">
+        <v>4.8807211514517654E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <v>99.918000000000006</v>
+      </c>
+      <c r="D56">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57">
+        <v>99.876999999999995</v>
+      </c>
+      <c r="D57">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58">
+        <v>99.549000000000007</v>
+      </c>
+      <c r="D58">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <v>84.828999999999994</v>
+      </c>
+      <c r="D59">
+        <v>2.3639999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>22.007999999999999</v>
+      </c>
+      <c r="D60">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>